<commit_message>
nutritional requirements preprocess finished
</commit_message>
<xml_diff>
--- a/data/ad_hoc_data/nutrient_match.xlsx
+++ b/data/ad_hoc_data/nutrient_match.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pol\git\food-basket-optimization-and-selection\data\ad_hoc_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pol.gil.figuerola\Documents\git\food-basket-cambodia-case-study\data\ad_hoc_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1749A4-D7D9-4360-A171-D993448D4A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F95DA3-BF0E-4C88-A06C-6A73BE95CB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nutrient_match" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Exact</t>
   </si>
@@ -34,181 +34,184 @@
     <t>Exact_requirement</t>
   </si>
   <si>
+    <t>Energy (kcal)</t>
+  </si>
+  <si>
+    <t>ENERC_KCAL</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Protein (g)</t>
+  </si>
+  <si>
+    <t>PROTCNT</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Fat (g)</t>
+  </si>
+  <si>
+    <t>FAT</t>
+  </si>
+  <si>
+    <t>FatMinPercent</t>
+  </si>
+  <si>
+    <t>FatMaxPercent</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>ULCalcium</t>
+  </si>
+  <si>
+    <t>FOLDFE</t>
+  </si>
+  <si>
+    <t>Folate</t>
+  </si>
+  <si>
+    <t>FEABS</t>
+  </si>
+  <si>
+    <t>IronAbsorbed</t>
+  </si>
+  <si>
+    <t>Iron (mg)</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>ULIron</t>
+  </si>
+  <si>
+    <t>Magnesium (mg)</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>Magnesium</t>
+  </si>
+  <si>
+    <t>Niacin (mg NE)</t>
+  </si>
+  <si>
+    <t>NIAEQ</t>
+  </si>
+  <si>
+    <t>Niacin</t>
+  </si>
+  <si>
+    <t>ULNiacin</t>
+  </si>
+  <si>
+    <t>PANTAC</t>
+  </si>
+  <si>
+    <t>PantothenicAcid</t>
+  </si>
+  <si>
+    <t>VITA_RAE</t>
+  </si>
+  <si>
+    <t>ULVitaminA</t>
+  </si>
+  <si>
+    <t>Vitamin B1 (mg)</t>
+  </si>
+  <si>
+    <t>THIA</t>
+  </si>
+  <si>
+    <t>VitaminB1</t>
+  </si>
+  <si>
+    <t>Vitamin B2 (mg)</t>
+  </si>
+  <si>
+    <t>RIBF</t>
+  </si>
+  <si>
+    <t>VitaminB2</t>
+  </si>
+  <si>
+    <t>Vitamin B6 (mg)</t>
+  </si>
+  <si>
+    <t>VITB6C</t>
+  </si>
+  <si>
+    <t>VitaminB6</t>
+  </si>
+  <si>
+    <t>VITB12</t>
+  </si>
+  <si>
+    <t>VitaminB12</t>
+  </si>
+  <si>
+    <t>Vitamin C (mg)</t>
+  </si>
+  <si>
+    <t>VITC</t>
+  </si>
+  <si>
+    <t>VitaminC</t>
+  </si>
+  <si>
+    <t>ULVitaminC</t>
+  </si>
+  <si>
+    <t>Zinc (mg)</t>
+  </si>
+  <si>
+    <t>ZN</t>
+  </si>
+  <si>
+    <t>ZincSemiunref</t>
+  </si>
+  <si>
+    <t>nutrient_name_food_composition</t>
+  </si>
+  <si>
+    <t>Calcium (mg)</t>
+  </si>
+  <si>
+    <t>Folic acid (µg DFE)</t>
+  </si>
+  <si>
+    <t>Iron absorbed (mg)</t>
+  </si>
+  <si>
+    <t>Pantothenic acid (mg)</t>
+  </si>
+  <si>
+    <t>Vitamin A (μg RAE)</t>
+  </si>
+  <si>
+    <t>Vitamin B12 (µg)</t>
+  </si>
+  <si>
+    <t>Nutrient</t>
+  </si>
+  <si>
     <t>Lower_limits</t>
   </si>
   <si>
     <t>Upper_limits</t>
   </si>
   <si>
-    <t>Energy (kcal)</t>
-  </si>
-  <si>
-    <t>ENERC_KCAL</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>Protein (g)</t>
-  </si>
-  <si>
-    <t>PROTCNT</t>
-  </si>
-  <si>
-    <t>Protein</t>
-  </si>
-  <si>
-    <t>Fat (g)</t>
-  </si>
-  <si>
-    <t>FAT</t>
-  </si>
-  <si>
-    <t>FatMinPercent</t>
-  </si>
-  <si>
-    <t>FatMaxPercent</t>
-  </si>
-  <si>
-    <t>Ca (mg)</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>Calcium</t>
-  </si>
-  <si>
-    <t>ULCalcium</t>
-  </si>
-  <si>
-    <t>FOLDFE</t>
-  </si>
-  <si>
-    <t>Folate</t>
-  </si>
-  <si>
-    <t>Iron Absorbed (mg)</t>
-  </si>
-  <si>
-    <t>FEABS</t>
-  </si>
-  <si>
-    <t>IronAbsorbed</t>
-  </si>
-  <si>
-    <t>Iron (mg)</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>ULIron</t>
-  </si>
-  <si>
-    <t>Magnesium (mg)</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>Magnesium</t>
-  </si>
-  <si>
-    <t>Niacin (mg NE)</t>
-  </si>
-  <si>
-    <t>NIAEQ</t>
-  </si>
-  <si>
-    <t>Niacin</t>
-  </si>
-  <si>
-    <t>ULNiacin</t>
-  </si>
-  <si>
-    <t>PantothenicAcid (mg)</t>
-  </si>
-  <si>
-    <t>PANTAC</t>
-  </si>
-  <si>
-    <t>PantothenicAcid</t>
-  </si>
-  <si>
-    <t>VITA_RAE</t>
-  </si>
-  <si>
-    <t>ULVitaminA</t>
-  </si>
-  <si>
-    <t>Vitamin B1 (mg)</t>
-  </si>
-  <si>
-    <t>THIA</t>
-  </si>
-  <si>
-    <t>VitaminB1</t>
-  </si>
-  <si>
-    <t>Vitamin B2 (mg)</t>
-  </si>
-  <si>
-    <t>RIBF</t>
-  </si>
-  <si>
-    <t>VitaminB2</t>
-  </si>
-  <si>
-    <t>Vitamin B6 (mg)</t>
-  </si>
-  <si>
-    <t>VITB6C</t>
-  </si>
-  <si>
-    <t>VitaminB6</t>
-  </si>
-  <si>
-    <t>VITB12</t>
-  </si>
-  <si>
-    <t>VitaminB12</t>
-  </si>
-  <si>
-    <t>Vitamin C (mg)</t>
-  </si>
-  <si>
-    <t>VITC</t>
-  </si>
-  <si>
-    <t>VitaminC</t>
-  </si>
-  <si>
-    <t>ULVitaminC</t>
-  </si>
-  <si>
-    <t>Zinc (mg)</t>
-  </si>
-  <si>
-    <t>ZN</t>
-  </si>
-  <si>
-    <t>ZincSemiunref</t>
-  </si>
-  <si>
-    <t>Vitamin A (Âug RE)</t>
-  </si>
-  <si>
-    <t>Vitamin B12(Âug)</t>
-  </si>
-  <si>
-    <t>FolicAcid (Âug DFE)</t>
-  </si>
-  <si>
-    <t>nutrient</t>
-  </si>
-  <si>
-    <t>nutrient_name_food_composition</t>
+    <t>RetinolActivityEquivalent</t>
   </si>
 </sst>
 </file>
@@ -694,7 +697,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,7 +1073,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,10 +1086,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1099,104 +1104,104 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="H4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -1208,15 +1213,15 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -1228,15 +1233,15 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -1248,15 +1253,15 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1268,15 +1273,15 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1288,18 +1293,18 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -1311,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1319,27 +1324,30 @@
         <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1351,15 +1359,15 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1371,15 +1379,15 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1391,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1399,7 +1407,7 @@
         <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -1411,15 +1419,15 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1431,18 +1439,18 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1454,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>